<commit_message>
edit show result pdf
</commit_message>
<xml_diff>
--- a/studentCourse.xlsx
+++ b/studentCourse.xlsx
@@ -22,7 +22,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>ssss</t>
+    <t>hossam</t>
   </si>
 </sst>
 </file>
@@ -361,15 +361,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -381,19 +381,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>159753</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>789456123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>789546</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>123456789053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>